<commit_message>
Made inverted index api and update the controller added a column name rankscore in laptop model
</commit_message>
<xml_diff>
--- a/src/main/resources/products-Excel.xlsx
+++ b/src/main/resources/products-Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\ACC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHARAD\Desktop\ACC CHAPTERS PPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A6298C-2BD4-475A-A96D-280EE7310EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B022FE8A-F959-48C6-9FB1-9ADDCAD19AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D6B59C98-8537-4701-B434-75DDBC406416}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6330" uniqueCount="1601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6331" uniqueCount="1602">
   <si>
     <t>ProductName</t>
   </si>
@@ -4823,6 +4823,9 @@
   </si>
   <si>
     <t>https://rog.asus.com/ca-en/laptops/rog-flow/2021-rog-flow-x13-series/</t>
+  </si>
+  <si>
+    <t>Rank</t>
   </si>
 </sst>
 </file>
@@ -5694,10 +5697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C068153E-CE61-4AE3-ACD6-6199127DD3CE}">
-  <dimension ref="A1:K628"/>
+  <dimension ref="A1:L628"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" zoomScale="105" workbookViewId="0">
-      <selection activeCell="K259" sqref="K259"/>
+    <sheetView tabSelected="1" topLeftCell="F241" zoomScale="105" workbookViewId="0">
+      <selection activeCell="L242" sqref="L242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5707,6 +5710,7 @@
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="31.33203125" customWidth="1"/>
     <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="99.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -13392,7 +13396,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>1466</v>
       </c>
@@ -13423,8 +13427,11 @@
       <c r="J241" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L241" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>1466</v>
       </c>
@@ -13456,7 +13463,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>1467</v>
       </c>
@@ -13491,7 +13498,7 @@
         <v>1555</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>1467</v>
       </c>
@@ -13526,7 +13533,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>1467</v>
       </c>
@@ -13561,7 +13568,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>1467</v>
       </c>
@@ -13596,7 +13603,7 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>1467</v>
       </c>
@@ -13631,7 +13638,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>1467</v>
       </c>
@@ -13666,7 +13673,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>1467</v>
       </c>
@@ -13701,7 +13708,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>1467</v>
       </c>
@@ -13736,7 +13743,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>1467</v>
       </c>
@@ -13771,7 +13778,7 @@
         <v>1563</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>1467</v>
       </c>
@@ -13806,7 +13813,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>1467</v>
       </c>
@@ -13841,7 +13848,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>1467</v>
       </c>
@@ -13876,7 +13883,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>1467</v>
       </c>
@@ -13911,7 +13918,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>1467</v>
       </c>

</xml_diff>